<commit_message>
Begin pricing/cost basis breakeven analysis
</commit_message>
<xml_diff>
--- a/explore/costs_calc.xlsx
+++ b/explore/costs_calc.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rime/uw-datascience/ds785/thesis_latex/explore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF61B0D5-79A1-E24B-960C-32B658FF29FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94ADD4B-9248-F541-BF60-852B8D4838FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="460" windowWidth="32300" windowHeight="19560" xr2:uid="{5F43299C-6689-8349-9F7B-1CAF92A64BB7}"/>
+    <workbookView xWindow="460" yWindow="460" windowWidth="41840" windowHeight="19560" activeTab="1" xr2:uid="{5F43299C-6689-8349-9F7B-1CAF92A64BB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Explorer" sheetId="1" r:id="rId1"/>
+    <sheet name="Pricing Cost Basis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>t</t>
   </si>
@@ -76,14 +77,145 @@
   </si>
   <si>
     <t>Concurrent Scan Limit:</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Enterprise</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>USERS</t>
+  </si>
+  <si>
+    <t>WEBSITES</t>
+  </si>
+  <si>
+    <t>PAGES</t>
+  </si>
+  <si>
+    <t>PROF.SERVICES</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>WEB HOOKS</t>
+  </si>
+  <si>
+    <t>NOTIFICATIONS</t>
+  </si>
+  <si>
+    <t>RECOMMENDATION</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>SCANS</t>
+  </si>
+  <si>
+    <t>Professional Services per Hour</t>
+  </si>
+  <si>
+    <t>EST Operations Cost / mo</t>
+  </si>
+  <si>
+    <t>Plan Cost / mo</t>
+  </si>
+  <si>
+    <t>Professional Services Cost per Hour</t>
+  </si>
+  <si>
+    <t>AVG Report Size/page (GB)</t>
+  </si>
+  <si>
+    <t>AVG WebHook Payload Size (GB)</t>
+  </si>
+  <si>
+    <t>S3 Cost/GB</t>
+  </si>
+  <si>
+    <t>ELB Cost/GB</t>
+  </si>
+  <si>
+    <t>ELB Cost/Req/Mil</t>
+  </si>
+  <si>
+    <t>Est API Req/mo/user</t>
+  </si>
+  <si>
+    <t>Network Cost/GB</t>
+  </si>
+  <si>
+    <t>Cloudfront Cost/GB</t>
+  </si>
+  <si>
+    <t>Cloudfront Traffic/User (GB)</t>
+  </si>
+  <si>
+    <t>Time ( 100 websites / n_plan )</t>
+  </si>
+  <si>
+    <t>Subscriptions:</t>
+  </si>
+  <si>
+    <t>Free:</t>
+  </si>
+  <si>
+    <t>Personal:</t>
+  </si>
+  <si>
+    <t>Professional:</t>
+  </si>
+  <si>
+    <t>Enterprise:</t>
+  </si>
+  <si>
+    <t>Price:</t>
+  </si>
+  <si>
+    <t>Profit/mo:</t>
+  </si>
+  <si>
+    <t>Margin:</t>
+  </si>
+  <si>
+    <t>Break Even:</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>W/O Prof Services</t>
+  </si>
+  <si>
+    <t>Max Plans Supported:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,8 +243,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4CF063-D35C-5B46-BFAD-CEE1E92E4454}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -550,4 +704,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EA282-AFBB-4F4A-8D47-8A0346E952E6}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" style="2" customWidth="1"/>
+    <col min="2" max="4" width="21.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="2" customWidth="1"/>
+    <col min="7" max="9" width="21.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="2" customWidth="1"/>
+    <col min="11" max="12" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <f>(((B16*(B2*G2))+(((B2*B14)/1000000)*B15)) + (B13*(C2*D2*E2*B12))+((B17 * (C2*D2*E2*B12)) + B13*(C2*D2*E2*B11) + (B18*B2*B19))) + (B22*F2)</f>
+        <v>0.10300179100000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <f>B9*(((B16*(B3*G3))+(((B3*B14)/1000000)*B15)) + (B13*(C3*D3*E3*B12))+((B17 * (C3*D3*E3*B12)) + B13*(C3*D3*E3*B11) + (B18*B3*B19))) + (B22*F3)</f>
+        <v>2.0601791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <f>B9*(((B16*(B4*G4))+(((B4*B14)/1000000)*B15)) + (B13*(C4*D4*E4*B12))+((B17 * (C4*D4*E4*B12)) + B13*(C4*D4*E4*B11) + (B18*B4*B19))) + (B22*F4)</f>
+        <v>10.308955000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <f>B9*(((B16*(B5*G5))+(((B5*B14)/1000000)*B15)) + (B13*(C5*D5*E5*B12))+((B17 * (C5*D5*E5*B12)) + B13*(C5*D5*E5*B11) + (B18*B5*B19))) + (B22*F5)</f>
+        <v>353.35820000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <f>B9*(((B16*(B5*G5))+(((B5*B14)/1000000)*B15)) + (B13*(C5*D5*E5*B12))+((B17 * (C5*D5*E5*B12)) + B13*(C5*D5*E5*B11) + (B18*B5*B19)))</f>
+        <v>55.858199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>157.13999999999999</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9-K2</f>
+        <v>-0.10300179100000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="2">
+        <f>100/C2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10-K3</f>
+        <v>36.939820900000001</v>
+      </c>
+      <c r="F10" s="2">
+        <f>E10/D10</f>
+        <v>0.94717489487179485</v>
+      </c>
+      <c r="G10" s="2">
+        <f>ROUNDUP(B8/E10, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <f>100/C3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1">
+        <v>99.99</v>
+      </c>
+      <c r="E11" s="2">
+        <f>D11-K4</f>
+        <v>89.681044999999997</v>
+      </c>
+      <c r="F11" s="2">
+        <f>E11/D11</f>
+        <v>0.89690014001400142</v>
+      </c>
+      <c r="G11" s="2">
+        <f>ROUNDUP(B8/E11, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <f>100/C4</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.5999999999999998E-5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1299</v>
+      </c>
+      <c r="E12" s="8">
+        <f>D12-K5</f>
+        <v>945.64179999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <f>E12/D12</f>
+        <v>0.72797675134719009</v>
+      </c>
+      <c r="G12" s="2">
+        <f>ROUNDUP(B8/E12, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <f>100/C5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add Cereus competitive overview
</commit_message>
<xml_diff>
--- a/explore/costs_calc.xlsx
+++ b/explore/costs_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rime/uw-datascience/ds785/thesis_latex/explore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874C3791-3758-474A-B418-EB6C718E2F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE280862-E7FE-1B49-A509-DCF9B9A2D357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1000" windowWidth="37460" windowHeight="19560" activeTab="1" xr2:uid="{5F43299C-6689-8349-9F7B-1CAF92A64BB7}"/>
+    <workbookView xWindow="1960" yWindow="2060" windowWidth="39000" windowHeight="19560" activeTab="1" xr2:uid="{5F43299C-6689-8349-9F7B-1CAF92A64BB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Explorer" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
     <t>Enterprise w/o Prof:</t>
   </si>
   <si>
-    <t>Prof web*scans baseline</t>
+    <t>Prof web*scans baseline ( C )</t>
   </si>
 </sst>
 </file>
@@ -3865,7 +3865,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>